<commit_message>
Xml files and folders hierarchy
</commit_message>
<xml_diff>
--- a/Exceldata/VHLFTF.xlsx
+++ b/Exceldata/VHLFTF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\latest\etraffic_CI\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9989107B-8153-4EF1-8067-653DE1CB457D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F437D756-98E9-472E-A27B-7C51E788EF83}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14655" windowHeight="2490" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14655" windowHeight="2490" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registration" sheetId="1" r:id="rId1"/>
@@ -1032,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CDEEFD-8C8E-45EE-B6B4-5440631457C5}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -2519,10 +2519,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B1673E-3475-424F-9FE6-30D87BC3F3E4}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,19 +2568,22 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>